<commit_message>
Ressourcen Planung erweitert. Ist-Soll Planung
</commit_message>
<xml_diff>
--- a/ressourcenplanung.xlsx
+++ b/ressourcenplanung.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="26">
   <si>
     <t>SW 1</t>
   </si>
@@ -64,9 +64,6 @@
     <t>Jedes Kästchen bedeutet 10 Arbeitsstunden</t>
   </si>
   <si>
-    <t>Gesamt</t>
-  </si>
-  <si>
     <t>140h</t>
   </si>
   <si>
@@ -83,6 +80,18 @@
   </si>
   <si>
     <t>Elektrotechnik</t>
+  </si>
+  <si>
+    <t>SOLL</t>
+  </si>
+  <si>
+    <t>IST</t>
+  </si>
+  <si>
+    <t>Gesamt SOLL</t>
+  </si>
+  <si>
+    <t>Gesamt IST</t>
   </si>
 </sst>
 </file>
@@ -146,7 +155,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -174,17 +183,6 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
       <top/>
       <bottom style="thin">
         <color indexed="64"/>
@@ -202,19 +200,6 @@
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -234,7 +219,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -242,25 +227,38 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -565,102 +563,88 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q13"/>
+  <dimension ref="A1:Q25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q11" sqref="Q11:Q13"/>
+      <selection activeCell="P7" sqref="P7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="14" width="8.28515625" customWidth="1"/>
+    <col min="15" max="15" width="4.5703125" customWidth="1"/>
     <col min="17" max="17" width="39.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="15" t="s">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A1" s="18" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="B2" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="15" t="s">
+      <c r="C2" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="15" t="s">
+      <c r="D2" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="15" t="s">
+      <c r="E2" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="15" t="s">
+      <c r="F2" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="15" t="s">
+      <c r="G2" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="15" t="s">
+      <c r="H2" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="15" t="s">
+      <c r="I2" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="15" t="s">
+      <c r="J2" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="15" t="s">
+      <c r="K2" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="15" t="s">
+      <c r="L2" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="15" t="s">
+      <c r="M2" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="16" t="s">
+      <c r="N2" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="17"/>
-      <c r="P1" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q1" s="6"/>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A2" s="11"/>
-      <c r="B2" s="11"/>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
-      <c r="F2" s="11"/>
-      <c r="G2" s="11"/>
-      <c r="H2" s="11"/>
-      <c r="I2" s="11"/>
-      <c r="J2" s="11"/>
-      <c r="K2" s="11"/>
-      <c r="L2" s="11"/>
-      <c r="M2" s="11"/>
-      <c r="N2" s="7"/>
+      <c r="O2" s="15"/>
+      <c r="P2" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q2" s="1"/>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A3" s="12"/>
-      <c r="B3" s="12"/>
-      <c r="C3" s="12"/>
-      <c r="D3" s="12"/>
-      <c r="E3" s="12"/>
-      <c r="F3" s="12"/>
-      <c r="G3" s="12"/>
-      <c r="H3" s="12"/>
-      <c r="I3" s="12"/>
-      <c r="J3" s="12"/>
-      <c r="K3" s="12"/>
-      <c r="L3" s="12"/>
-      <c r="M3" s="12"/>
-      <c r="N3" s="8"/>
-      <c r="P3" s="18"/>
-      <c r="Q3" t="s">
-        <v>15</v>
-      </c>
+      <c r="A3" s="11"/>
+      <c r="B3" s="11"/>
+      <c r="C3" s="11"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="11"/>
+      <c r="F3" s="11"/>
+      <c r="G3" s="11"/>
+      <c r="H3" s="11"/>
+      <c r="I3" s="11"/>
+      <c r="J3" s="11"/>
+      <c r="K3" s="11"/>
+      <c r="L3" s="11"/>
+      <c r="M3" s="11"/>
+      <c r="N3" s="7"/>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="12"/>
@@ -677,45 +661,55 @@
       <c r="L4" s="12"/>
       <c r="M4" s="12"/>
       <c r="N4" s="8"/>
+      <c r="P4" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A5" s="13"/>
-      <c r="B5" s="13"/>
-      <c r="C5" s="13"/>
-      <c r="D5" s="13"/>
-      <c r="E5" s="13"/>
-      <c r="F5" s="13"/>
-      <c r="G5" s="13"/>
-      <c r="H5" s="13"/>
-      <c r="I5" s="13"/>
-      <c r="J5" s="13"/>
-      <c r="K5" s="13"/>
-      <c r="L5" s="13"/>
-      <c r="M5" s="13"/>
-      <c r="N5" s="9"/>
-      <c r="P5" s="2"/>
+      <c r="A5" s="12"/>
+      <c r="B5" s="12"/>
+      <c r="C5" s="12"/>
+      <c r="D5" s="12"/>
+      <c r="E5" s="12"/>
+      <c r="F5" s="12"/>
+      <c r="G5" s="12"/>
+      <c r="H5" s="12"/>
+      <c r="I5" s="12"/>
+      <c r="J5" s="12"/>
+      <c r="K5" s="12"/>
+      <c r="L5" s="12"/>
+      <c r="M5" s="12"/>
+      <c r="N5" s="8"/>
+      <c r="P5" s="17" t="s">
+        <v>17</v>
+      </c>
       <c r="Q5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A6" s="14"/>
-      <c r="B6" s="14"/>
-      <c r="C6" s="14"/>
-      <c r="D6" s="14"/>
-      <c r="E6" s="14"/>
-      <c r="F6" s="14"/>
-      <c r="G6" s="14"/>
-      <c r="H6" s="14"/>
-      <c r="I6" s="14"/>
-      <c r="J6" s="14"/>
-      <c r="K6" s="14"/>
-      <c r="L6" s="14"/>
-      <c r="M6" s="14"/>
-      <c r="N6" s="10"/>
-      <c r="P6" s="3"/>
+      <c r="A6" s="13"/>
+      <c r="B6" s="13"/>
+      <c r="C6" s="13"/>
+      <c r="D6" s="13"/>
+      <c r="E6" s="13"/>
+      <c r="F6" s="13"/>
+      <c r="G6" s="13"/>
+      <c r="H6" s="13"/>
+      <c r="I6" s="13"/>
+      <c r="J6" s="13"/>
+      <c r="K6" s="13"/>
+      <c r="L6" s="13"/>
+      <c r="M6" s="13"/>
+      <c r="N6" s="9"/>
+      <c r="P6" s="17" t="s">
+        <v>18</v>
+      </c>
       <c r="Q6" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
@@ -733,43 +727,222 @@
       <c r="L7" s="14"/>
       <c r="M7" s="14"/>
       <c r="N7" s="10"/>
-      <c r="P7" s="4"/>
-      <c r="Q7" t="s">
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A8" s="14"/>
+      <c r="B8" s="14"/>
+      <c r="C8" s="14"/>
+      <c r="D8" s="14"/>
+      <c r="E8" s="14"/>
+      <c r="F8" s="14"/>
+      <c r="G8" s="14"/>
+      <c r="H8" s="14"/>
+      <c r="I8" s="14"/>
+      <c r="J8" s="14"/>
+      <c r="K8" s="14"/>
+      <c r="L8" s="14"/>
+      <c r="M8" s="14"/>
+      <c r="N8" s="10"/>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A10" s="18" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A11" s="27" t="s">
+        <v>0</v>
+      </c>
+      <c r="B11" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="C11" s="27" t="s">
+        <v>2</v>
+      </c>
+      <c r="D11" s="27" t="s">
+        <v>3</v>
+      </c>
+      <c r="E11" s="27" t="s">
+        <v>4</v>
+      </c>
+      <c r="F11" s="27" t="s">
+        <v>5</v>
+      </c>
+      <c r="G11" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="H11" s="27" t="s">
+        <v>7</v>
+      </c>
+      <c r="I11" s="27" t="s">
+        <v>8</v>
+      </c>
+      <c r="J11" s="27" t="s">
+        <v>9</v>
+      </c>
+      <c r="K11" s="27" t="s">
+        <v>10</v>
+      </c>
+      <c r="L11" s="27" t="s">
+        <v>11</v>
+      </c>
+      <c r="M11" s="27" t="s">
+        <v>12</v>
+      </c>
+      <c r="N11" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="P11" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q11" s="1"/>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A12" s="11"/>
+      <c r="B12" s="11"/>
+      <c r="C12" s="19"/>
+      <c r="D12" s="19"/>
+      <c r="E12" s="19"/>
+      <c r="F12" s="19"/>
+      <c r="G12" s="19"/>
+      <c r="H12" s="19"/>
+      <c r="I12" s="19"/>
+      <c r="J12" s="19"/>
+      <c r="K12" s="19"/>
+      <c r="L12" s="19"/>
+      <c r="M12" s="19"/>
+      <c r="N12" s="20"/>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A13" s="12"/>
+      <c r="B13" s="12"/>
+      <c r="C13" s="21"/>
+      <c r="D13" s="21"/>
+      <c r="E13" s="21"/>
+      <c r="F13" s="21"/>
+      <c r="G13" s="21"/>
+      <c r="H13" s="21"/>
+      <c r="I13" s="21"/>
+      <c r="J13" s="21"/>
+      <c r="K13" s="21"/>
+      <c r="L13" s="21"/>
+      <c r="M13" s="21"/>
+      <c r="N13" s="22"/>
+      <c r="P13" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q13" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A14" s="12"/>
+      <c r="B14" s="12"/>
+      <c r="C14" s="21"/>
+      <c r="D14" s="21"/>
+      <c r="E14" s="21"/>
+      <c r="F14" s="21"/>
+      <c r="G14" s="21"/>
+      <c r="H14" s="21"/>
+      <c r="I14" s="21"/>
+      <c r="J14" s="21"/>
+      <c r="K14" s="21"/>
+      <c r="L14" s="21"/>
+      <c r="M14" s="21"/>
+      <c r="N14" s="22"/>
+      <c r="P14" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q14" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="P9" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q9" s="1"/>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="P11" s="19" t="s">
-        <v>17</v>
-      </c>
-      <c r="Q11" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="P12" s="19" t="s">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A15" s="13"/>
+      <c r="B15" s="13"/>
+      <c r="C15" s="23"/>
+      <c r="D15" s="23"/>
+      <c r="E15" s="23"/>
+      <c r="F15" s="23"/>
+      <c r="G15" s="23"/>
+      <c r="H15" s="23"/>
+      <c r="I15" s="23"/>
+      <c r="J15" s="23"/>
+      <c r="K15" s="23"/>
+      <c r="L15" s="23"/>
+      <c r="M15" s="23"/>
+      <c r="N15" s="24"/>
+      <c r="P15" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="Q12" t="s">
+      <c r="Q15" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A16" s="14"/>
+      <c r="B16" s="14"/>
+      <c r="C16" s="25"/>
+      <c r="D16" s="25"/>
+      <c r="E16" s="25"/>
+      <c r="F16" s="25"/>
+      <c r="G16" s="25"/>
+      <c r="H16" s="25"/>
+      <c r="I16" s="25"/>
+      <c r="J16" s="25"/>
+      <c r="K16" s="25"/>
+      <c r="L16" s="25"/>
+      <c r="M16" s="25"/>
+      <c r="N16" s="26"/>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A17" s="14"/>
+      <c r="B17" s="14"/>
+      <c r="C17" s="25"/>
+      <c r="D17" s="25"/>
+      <c r="E17" s="25"/>
+      <c r="F17" s="25"/>
+      <c r="G17" s="25"/>
+      <c r="H17" s="25"/>
+      <c r="I17" s="25"/>
+      <c r="J17" s="25"/>
+      <c r="K17" s="25"/>
+      <c r="L17" s="25"/>
+      <c r="M17" s="25"/>
+      <c r="N17" s="26"/>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="P19" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q19" s="6"/>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="P21" s="16"/>
+      <c r="Q21" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="P23" s="2"/>
+      <c r="Q23" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="P13" s="19" t="s">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="P24" s="3"/>
+      <c r="Q24" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="P25" s="4"/>
+      <c r="Q25" t="s">
         <v>19</v>
-      </c>
-      <c r="Q13" t="s">
-        <v>20</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>